<commit_message>
code generator tool update
</commit_message>
<xml_diff>
--- a/config/excel/hero.xlsx
+++ b/config/excel/hero.xlsx
@@ -19,15 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>AppType.ClientH |  AppType.ClientM | AppType.Gate</t>
   </si>
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>#测试说明</t>
   </si>
   <si>
     <t>名字</t>
@@ -216,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -224,11 +221,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -238,9 +231,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1439,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1450,14 +1440,13 @@
     <col min="1" max="1" width="61.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="21.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="4" max="4" width="9.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="21.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1467,9 +1456,8 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -1477,15 +1465,16 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1493,13 +1482,10 @@
         <v>7</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
@@ -1515,90 +1501,83 @@
         <v>4</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7"/>
       <c r="E5" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="15">
+      <c r="D6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="12">
         <v>2</v>
       </c>
-      <c r="G6" s="12">
+      <c r="F6" s="10">
         <v>1</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>18</v>
+      <c r="G6" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>2</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="11">
+      <c r="D7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="9">
         <v>3</v>
       </c>
-      <c r="G7" s="8">
+      <c r="F7" s="7">
         <v>0</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>19</v>
+      <c r="G7" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>3</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="11">
+      <c r="D8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9">
         <v>4</v>
       </c>
-      <c r="G8" s="8">
+      <c r="F8" s="7">
         <v>2</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>20</v>
+      <c r="G8" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel parser bug fix
</commit_message>
<xml_diff>
--- a/config/excel/hero.xlsx
+++ b/config/excel/hero.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
-  <si>
-    <t>AppType.ClientH |  AppType.ClientM | AppType.Gate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -64,35 +61,47 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>属性列表</t>
+    <t>default</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>AttList</t>
+    <t>-1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>int[]</t>
+    <t>0</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>1,2,3</t>
+    <t>行列头两行不会被读取</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>0,7,8</t>
+    <t>默认英雄名</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>22,993,17,31</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>导出字段描述</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>导出字段名</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>导出字段类型</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>导出字段默认值</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -119,6 +128,27 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Helvetica Neue"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -140,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -177,19 +207,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -216,11 +233,9 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -230,15 +245,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1429,155 +1446,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="61.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="21.5" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="16.149999999999999" customHeight="1">
+      <c r="A1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.149999999999999" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="16.149999999999999" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.149999999999999" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+    <row r="5" spans="1:6" ht="16.149999999999999" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
+    <row r="6" spans="1:6" ht="16.149999999999999" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
+    <row r="7" spans="1:6" ht="14.65" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="8">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.65" customHeight="1">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="D8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7">
         <v>3</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.65" customHeight="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="5">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7">
         <v>4</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="10">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="F9" s="5">
         <v>2</v>
-      </c>
-      <c r="F6" s="10">
-        <v>1</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="9">
-        <v>3</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="7">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="9">
-        <v>4</v>
-      </c>
-      <c r="F8" s="7">
-        <v>2</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>